<commit_message>
for JD AOS testing.
</commit_message>
<xml_diff>
--- a/POC Sample Allocation.xlsx
+++ b/POC Sample Allocation.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guohao/Library/Containers/com.apple.mail/Data/Library/Mail Downloads/D697DB36-77FB-4540-8765-E900846E9CF6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guohao/Works/OfficeAffairs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22200"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14660"/>
   </bookViews>
   <sheets>
     <sheet name="3. POC Sample Tracking" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
   <si>
     <r>
       <rPr>
@@ -707,6 +707,10 @@
     <rPh sb="0" eb="1">
       <t>liu hai jie</t>
     </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hanjianfei@jd.com</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -717,13 +721,13 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="DengXian"/>
       <family val="2"/>
-      <charset val="136"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -831,6 +835,15 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="DengXian"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -900,14 +913,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -977,6 +993,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -989,12 +1008,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8"/>
     <cellStyle name="千分位 2" xfId="1"/>
     <cellStyle name="一般 3" xfId="2"/>
   </cellStyles>
@@ -1329,7 +1349,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
+      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1510,6 +1530,9 @@
       <c r="K6" s="6" t="s">
         <v>71</v>
       </c>
+      <c r="L6" s="28" t="s">
+        <v>74</v>
+      </c>
       <c r="N6" s="14" t="s">
         <v>37</v>
       </c>
@@ -1544,6 +1567,9 @@
       </c>
       <c r="K7" s="6" t="s">
         <v>71</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>74</v>
       </c>
       <c r="N7" s="14" t="s">
         <v>37</v>
@@ -1776,8 +1802,12 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="L6" r:id="rId1"/>
+    <hyperlink ref="L7" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1819,14 +1849,14 @@
       <c r="F3" s="22"/>
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="22"/>
@@ -1845,46 +1875,46 @@
       <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
     </row>
     <row r="12" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
@@ -1947,94 +1977,94 @@
       <c r="F17" s="18"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="23"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="23"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="23"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="23"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="23"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="23"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -2134,11 +2164,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A7:F8"/>
-    <mergeCell ref="A21:F22"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="A1:F3"/>
@@ -2155,6 +2180,11 @@
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A7:F8"/>
+    <mergeCell ref="A21:F22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>